<commit_message>
Add NSW additional Anzac Day observance (2026+)
Calculate Anzac Day once and add an "Anzac Day (additional)" holiday for NSW from 2026 onward when the holiday falls on Saturday (observed Mon 27 Apr) or Sunday (observed Mon 26 Apr). Updated Holidays_NSW.cs to yield the extra dates and refreshed related test fixtures and snapshots (HTML, PNG, CSV, JSON, XML, ICS, Markdown, and verified text files) to reflect the new observance.
</commit_message>
<xml_diff>
--- a/src/Tests/Tests.ExportToExcelMultiState.verified.xlsx
+++ b/src/Tests/Tests.ExportToExcelMultiState.verified.xlsx
@@ -328,7 +328,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-06-08</t>
+          <t>2026-04-27</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -338,7 +338,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day (additional)</t>
         </is>
       </c>
     </row>
@@ -350,7 +350,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -362,85 +362,85 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-08-03</t>
+          <t>2026-06-08</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-09-25</t>
+          <t>2026-08-03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-10-05</t>
+          <t>2026-09-25</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-11-03</t>
+          <t>2026-10-05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-12-25</t>
+          <t>2026-11-03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
@@ -452,7 +452,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -464,17 +464,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-12-26</t>
+          <t>2026-12-25</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -498,17 +498,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-12-28</t>
+          <t>2026-12-26</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Christmas (additional)</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -532,17 +532,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2027-01-01</t>
+          <t>2026-12-28</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Christmas (additional)</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -566,17 +566,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2027-01-26</t>
+          <t>2027-01-01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -600,7 +600,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2027-03-08</t>
+          <t>2027-01-26</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -610,24 +610,24 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2027-03-26</t>
+          <t>2027-03-08</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -651,17 +651,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2027-03-27</t>
+          <t>2027-03-26</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -685,17 +685,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2027-03-28</t>
+          <t>2027-03-27</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -719,17 +719,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2027-03-29</t>
+          <t>2027-03-28</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -753,17 +753,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2027-04-25</t>
+          <t>2027-03-29</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
@@ -775,7 +775,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -787,41 +787,41 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2027-06-14</t>
+          <t>2027-04-25</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2027-06-14</t>
+          <t>2027-04-26</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day (additional)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2027-08-02</t>
+          <t>2027-06-14</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -831,14 +831,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2027-09-24</t>
+          <t>2027-06-14</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -848,14 +848,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2027-10-04</t>
+          <t>2027-08-02</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -865,14 +865,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2027-11-02</t>
+          <t>2027-09-24</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -882,14 +882,14 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2027-12-25</t>
+          <t>2027-10-04</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -899,14 +899,14 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2027-12-25</t>
+          <t>2027-11-02</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -916,14 +916,14 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2027-12-26</t>
+          <t>2027-12-25</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -933,14 +933,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2027-12-26</t>
+          <t>2027-12-25</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -950,14 +950,14 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2027-12-27</t>
+          <t>2027-12-26</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -967,14 +967,14 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Christmas (additional)</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2027-12-27</t>
+          <t>2027-12-26</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -984,14 +984,14 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Christmas (additional)</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2027-12-28</t>
+          <t>2027-12-27</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2027-12-28</t>
+          <t>2027-12-27</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1025,7 +1025,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2028-01-01</t>
+          <t>2027-12-28</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1035,14 +1035,14 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Christmas (additional)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2028-01-01</t>
+          <t>2027-12-28</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1052,14 +1052,14 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Christmas (additional)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2028-01-03</t>
+          <t>2028-01-01</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1069,82 +1069,82 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>New Year's Day (additional)</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2028-01-26</t>
+          <t>2028-01-01</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2028-01-26</t>
+          <t>2028-01-03</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day (additional)</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2028-03-13</t>
+          <t>2028-01-26</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2028-04-14</t>
+          <t>2028-01-26</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2028-04-14</t>
+          <t>2028-03-13</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1154,14 +1154,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2028-04-15</t>
+          <t>2028-04-14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1171,14 +1171,14 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2028-04-15</t>
+          <t>2028-04-14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1188,14 +1188,14 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2028-04-16</t>
+          <t>2028-04-15</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1205,14 +1205,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2028-04-16</t>
+          <t>2028-04-15</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1222,14 +1222,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2028-04-17</t>
+          <t>2028-04-16</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1239,14 +1239,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2028-04-17</t>
+          <t>2028-04-16</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1256,14 +1256,14 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2028-04-25</t>
+          <t>2028-04-17</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1273,14 +1273,14 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2028-04-25</t>
+          <t>2028-04-17</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1290,14 +1290,14 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2028-06-12</t>
+          <t>2028-04-25</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1307,14 +1307,14 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2028-06-12</t>
+          <t>2028-04-25</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1324,14 +1324,14 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2028-08-07</t>
+          <t>2028-06-12</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1341,14 +1341,14 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2028-09-29</t>
+          <t>2028-06-12</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1358,14 +1358,14 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2028-10-02</t>
+          <t>2028-08-07</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1375,14 +1375,14 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2028-11-07</t>
+          <t>2028-09-29</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1392,14 +1392,14 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2028-12-25</t>
+          <t>2028-10-02</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1409,14 +1409,14 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2028-12-25</t>
+          <t>2028-11-07</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1426,14 +1426,14 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2028-12-26</t>
+          <t>2028-12-25</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1443,14 +1443,14 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2028-12-26</t>
+          <t>2028-12-25</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1460,14 +1460,14 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2029-01-01</t>
+          <t>2028-12-26</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1477,14 +1477,14 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2029-01-01</t>
+          <t>2028-12-26</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1494,14 +1494,14 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2029-01-26</t>
+          <t>2029-01-01</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1511,14 +1511,14 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2029-01-26</t>
+          <t>2029-01-01</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1528,48 +1528,48 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2029-03-12</t>
+          <t>2029-01-26</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2029-03-30</t>
+          <t>2029-01-26</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2029-03-30</t>
+          <t>2029-03-12</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1579,14 +1579,14 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2029-03-31</t>
+          <t>2029-03-30</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1596,14 +1596,14 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2029-03-31</t>
+          <t>2029-03-30</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1613,14 +1613,14 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2029-04-01</t>
+          <t>2029-03-31</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1630,14 +1630,14 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2029-04-01</t>
+          <t>2029-03-31</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1647,14 +1647,14 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2029-04-02</t>
+          <t>2029-04-01</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1664,14 +1664,14 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2029-04-02</t>
+          <t>2029-04-01</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1681,14 +1681,14 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2029-04-25</t>
+          <t>2029-04-02</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1698,14 +1698,14 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2029-04-25</t>
+          <t>2029-04-02</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1715,14 +1715,14 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2029-06-11</t>
+          <t>2029-04-25</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1732,14 +1732,14 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2029-06-11</t>
+          <t>2029-04-25</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1749,14 +1749,14 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2029-08-06</t>
+          <t>2029-06-11</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1766,14 +1766,14 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2029-09-28</t>
+          <t>2029-06-11</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1783,14 +1783,14 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2029-10-01</t>
+          <t>2029-08-06</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1800,14 +1800,14 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2029-11-06</t>
+          <t>2029-09-28</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1817,14 +1817,14 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2029-12-25</t>
+          <t>2029-10-01</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1834,14 +1834,14 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2029-12-25</t>
+          <t>2029-11-06</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1851,14 +1851,14 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2029-12-26</t>
+          <t>2029-12-25</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1868,14 +1868,14 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2029-12-26</t>
+          <t>2029-12-25</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1885,14 +1885,14 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2030-01-01</t>
+          <t>2029-12-26</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1902,14 +1902,14 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2030-01-01</t>
+          <t>2029-12-26</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -1919,14 +1919,14 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2030-01-28</t>
+          <t>2030-01-01</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1936,14 +1936,14 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Australia Day (observed)</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2030-01-28</t>
+          <t>2030-01-01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1953,48 +1953,48 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Australia Day (observed)</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2030-03-11</t>
+          <t>2030-01-28</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day (observed)</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2030-04-19</t>
+          <t>2030-01-28</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Australia Day (observed)</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2030-04-19</t>
+          <t>2030-03-11</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2004,14 +2004,14 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2030-04-20</t>
+          <t>2030-04-19</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2021,14 +2021,14 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2030-04-20</t>
+          <t>2030-04-19</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2038,14 +2038,14 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2030-04-21</t>
+          <t>2030-04-20</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2055,14 +2055,14 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2030-04-21</t>
+          <t>2030-04-20</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2072,14 +2072,14 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2030-04-22</t>
+          <t>2030-04-21</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2089,14 +2089,14 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2030-04-22</t>
+          <t>2030-04-21</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2106,14 +2106,14 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2030-04-25</t>
+          <t>2030-04-22</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2123,14 +2123,14 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2030-04-25</t>
+          <t>2030-04-22</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2140,14 +2140,14 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2030-06-10</t>
+          <t>2030-04-25</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2157,14 +2157,14 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2030-06-10</t>
+          <t>2030-04-25</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2174,14 +2174,14 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2030-08-05</t>
+          <t>2030-06-10</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -2191,14 +2191,14 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2030-09-27</t>
+          <t>2030-06-10</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -2208,14 +2208,14 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2030-10-07</t>
+          <t>2030-08-05</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -2225,14 +2225,14 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2030-11-05</t>
+          <t>2030-09-27</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -2242,14 +2242,14 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2030-12-25</t>
+          <t>2030-10-07</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2259,14 +2259,14 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2030-12-25</t>
+          <t>2030-11-05</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -2276,14 +2276,14 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2030-12-26</t>
+          <t>2030-12-25</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2293,22 +2293,56 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
+          <t>2030-12-25</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>VIC</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Christmas Day</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
           <t>2030-12-26</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>VIC</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>NSW</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Boxing Day</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2030-12-26</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>VIC</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
         <is>
           <t>Boxing Day</t>
         </is>

</xml_diff>

<commit_message>
Add nsw additional anzac day observance (#18)
* Add NSW additional Anzac Day observance (2026+)

Calculate Anzac Day once and add an "Anzac Day (additional)" holiday for NSW from 2026 onward when the holiday falls on Saturday (observed Mon 27 Apr) or Sunday (observed Mon 26 Apr). Updated Holidays_NSW.cs to yield the extra dates and refreshed related test fixtures and snapshots (HTML, PNG, CSV, JSON, XML, ICS, Markdown, and verified text files) to reflect the new observance.

* .
</commit_message>
<xml_diff>
--- a/src/Tests/Tests.ExportToExcelMultiState.verified.xlsx
+++ b/src/Tests/Tests.ExportToExcelMultiState.verified.xlsx
@@ -328,7 +328,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-06-08</t>
+          <t>2026-04-27</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -338,7 +338,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day (additional)</t>
         </is>
       </c>
     </row>
@@ -350,7 +350,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -362,85 +362,85 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-08-03</t>
+          <t>2026-06-08</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-09-25</t>
+          <t>2026-08-03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-10-05</t>
+          <t>2026-09-25</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-11-03</t>
+          <t>2026-10-05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-12-25</t>
+          <t>2026-11-03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
@@ -452,7 +452,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -464,17 +464,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-12-26</t>
+          <t>2026-12-25</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -498,17 +498,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-12-28</t>
+          <t>2026-12-26</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Christmas (additional)</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -532,17 +532,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2027-01-01</t>
+          <t>2026-12-28</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Christmas (additional)</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -566,17 +566,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2027-01-26</t>
+          <t>2027-01-01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -600,7 +600,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2027-03-08</t>
+          <t>2027-01-26</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -610,24 +610,24 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2027-03-26</t>
+          <t>2027-03-08</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -651,17 +651,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2027-03-27</t>
+          <t>2027-03-26</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -685,17 +685,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2027-03-28</t>
+          <t>2027-03-27</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -719,17 +719,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2027-03-29</t>
+          <t>2027-03-28</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -753,17 +753,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2027-04-25</t>
+          <t>2027-03-29</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
@@ -775,7 +775,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -787,41 +787,41 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2027-06-14</t>
+          <t>2027-04-25</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2027-06-14</t>
+          <t>2027-04-26</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day (additional)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2027-08-02</t>
+          <t>2027-06-14</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -831,14 +831,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2027-09-24</t>
+          <t>2027-06-14</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -848,14 +848,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2027-10-04</t>
+          <t>2027-08-02</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -865,14 +865,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2027-11-02</t>
+          <t>2027-09-24</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -882,14 +882,14 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2027-12-25</t>
+          <t>2027-10-04</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -899,14 +899,14 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2027-12-25</t>
+          <t>2027-11-02</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -916,14 +916,14 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2027-12-26</t>
+          <t>2027-12-25</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -933,14 +933,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2027-12-26</t>
+          <t>2027-12-25</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -950,14 +950,14 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2027-12-27</t>
+          <t>2027-12-26</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -967,14 +967,14 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Christmas (additional)</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2027-12-27</t>
+          <t>2027-12-26</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -984,14 +984,14 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Christmas (additional)</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2027-12-28</t>
+          <t>2027-12-27</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2027-12-28</t>
+          <t>2027-12-27</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1025,7 +1025,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2028-01-01</t>
+          <t>2027-12-28</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1035,14 +1035,14 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Christmas (additional)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2028-01-01</t>
+          <t>2027-12-28</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1052,14 +1052,14 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Christmas (additional)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2028-01-03</t>
+          <t>2028-01-01</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1069,82 +1069,82 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>New Year's Day (additional)</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2028-01-26</t>
+          <t>2028-01-01</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2028-01-26</t>
+          <t>2028-01-03</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day (additional)</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2028-03-13</t>
+          <t>2028-01-26</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2028-04-14</t>
+          <t>2028-01-26</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2028-04-14</t>
+          <t>2028-03-13</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1154,14 +1154,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2028-04-15</t>
+          <t>2028-04-14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1171,14 +1171,14 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2028-04-15</t>
+          <t>2028-04-14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1188,14 +1188,14 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2028-04-16</t>
+          <t>2028-04-15</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1205,14 +1205,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2028-04-16</t>
+          <t>2028-04-15</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1222,14 +1222,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2028-04-17</t>
+          <t>2028-04-16</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1239,14 +1239,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2028-04-17</t>
+          <t>2028-04-16</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1256,14 +1256,14 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2028-04-25</t>
+          <t>2028-04-17</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1273,14 +1273,14 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2028-04-25</t>
+          <t>2028-04-17</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1290,14 +1290,14 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2028-06-12</t>
+          <t>2028-04-25</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1307,14 +1307,14 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2028-06-12</t>
+          <t>2028-04-25</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1324,14 +1324,14 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2028-08-07</t>
+          <t>2028-06-12</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1341,14 +1341,14 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2028-09-29</t>
+          <t>2028-06-12</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1358,14 +1358,14 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2028-10-02</t>
+          <t>2028-08-07</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1375,14 +1375,14 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2028-11-07</t>
+          <t>2028-09-29</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1392,14 +1392,14 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2028-12-25</t>
+          <t>2028-10-02</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1409,14 +1409,14 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2028-12-25</t>
+          <t>2028-11-07</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1426,14 +1426,14 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2028-12-26</t>
+          <t>2028-12-25</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1443,14 +1443,14 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2028-12-26</t>
+          <t>2028-12-25</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1460,14 +1460,14 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2029-01-01</t>
+          <t>2028-12-26</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1477,14 +1477,14 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2029-01-01</t>
+          <t>2028-12-26</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1494,14 +1494,14 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2029-01-26</t>
+          <t>2029-01-01</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1511,14 +1511,14 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2029-01-26</t>
+          <t>2029-01-01</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1528,48 +1528,48 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Australia Day</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2029-03-12</t>
+          <t>2029-01-26</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2029-03-30</t>
+          <t>2029-01-26</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Australia Day</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2029-03-30</t>
+          <t>2029-03-12</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1579,14 +1579,14 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2029-03-31</t>
+          <t>2029-03-30</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1596,14 +1596,14 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2029-03-31</t>
+          <t>2029-03-30</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1613,14 +1613,14 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2029-04-01</t>
+          <t>2029-03-31</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1630,14 +1630,14 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2029-04-01</t>
+          <t>2029-03-31</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1647,14 +1647,14 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2029-04-02</t>
+          <t>2029-04-01</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1664,14 +1664,14 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2029-04-02</t>
+          <t>2029-04-01</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1681,14 +1681,14 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2029-04-25</t>
+          <t>2029-04-02</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1698,14 +1698,14 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2029-04-25</t>
+          <t>2029-04-02</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1715,14 +1715,14 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2029-06-11</t>
+          <t>2029-04-25</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1732,14 +1732,14 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2029-06-11</t>
+          <t>2029-04-25</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1749,14 +1749,14 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2029-08-06</t>
+          <t>2029-06-11</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1766,14 +1766,14 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2029-09-28</t>
+          <t>2029-06-11</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1783,14 +1783,14 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2029-10-01</t>
+          <t>2029-08-06</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1800,14 +1800,14 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2029-11-06</t>
+          <t>2029-09-28</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1817,14 +1817,14 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2029-12-25</t>
+          <t>2029-10-01</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1834,14 +1834,14 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2029-12-25</t>
+          <t>2029-11-06</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1851,14 +1851,14 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2029-12-26</t>
+          <t>2029-12-25</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1868,14 +1868,14 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2029-12-26</t>
+          <t>2029-12-25</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1885,14 +1885,14 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2030-01-01</t>
+          <t>2029-12-26</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1902,14 +1902,14 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2030-01-01</t>
+          <t>2029-12-26</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -1919,14 +1919,14 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>New Year's Day</t>
+          <t>Boxing Day</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2030-01-28</t>
+          <t>2030-01-01</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1936,14 +1936,14 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Australia Day (observed)</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2030-01-28</t>
+          <t>2030-01-01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1953,48 +1953,48 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Australia Day (observed)</t>
+          <t>New Year's Day</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2030-03-11</t>
+          <t>2030-01-28</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>NSW</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Australia Day (observed)</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2030-04-19</t>
+          <t>2030-01-28</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>NSW</t>
+          <t>VIC</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Australia Day (observed)</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2030-04-19</t>
+          <t>2030-03-11</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2004,14 +2004,14 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Good Friday</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2030-04-20</t>
+          <t>2030-04-19</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2021,14 +2021,14 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2030-04-20</t>
+          <t>2030-04-19</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2038,14 +2038,14 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Easter Saturday</t>
+          <t>Good Friday</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2030-04-21</t>
+          <t>2030-04-20</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2055,14 +2055,14 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2030-04-21</t>
+          <t>2030-04-20</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2072,14 +2072,14 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Easter Sunday</t>
+          <t>Easter Saturday</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2030-04-22</t>
+          <t>2030-04-21</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2089,14 +2089,14 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2030-04-22</t>
+          <t>2030-04-21</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2106,14 +2106,14 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Easter Monday</t>
+          <t>Easter Sunday</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2030-04-25</t>
+          <t>2030-04-22</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2123,14 +2123,14 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2030-04-25</t>
+          <t>2030-04-22</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2140,14 +2140,14 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Anzac Day</t>
+          <t>Easter Monday</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2030-06-10</t>
+          <t>2030-04-25</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2157,14 +2157,14 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2030-06-10</t>
+          <t>2030-04-25</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2174,14 +2174,14 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>King's Birthday</t>
+          <t>Anzac Day</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2030-08-05</t>
+          <t>2030-06-10</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -2191,14 +2191,14 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Bank Holiday</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2030-09-27</t>
+          <t>2030-06-10</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -2208,14 +2208,14 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Friday before AFL Final (Subject to AFL schedule)</t>
+          <t>King's Birthday</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2030-10-07</t>
+          <t>2030-08-05</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -2225,14 +2225,14 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Labour Day</t>
+          <t>Bank Holiday</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2030-11-05</t>
+          <t>2030-09-27</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -2242,14 +2242,14 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Melbourne Cup Day</t>
+          <t>Friday before AFL Final (Subject to AFL schedule)</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2030-12-25</t>
+          <t>2030-10-07</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2259,14 +2259,14 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Labour Day</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2030-12-25</t>
+          <t>2030-11-05</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -2276,14 +2276,14 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Christmas Day</t>
+          <t>Melbourne Cup Day</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2030-12-26</t>
+          <t>2030-12-25</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2293,22 +2293,56 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Boxing Day</t>
+          <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
+          <t>2030-12-25</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>VIC</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Christmas Day</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
           <t>2030-12-26</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>VIC</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>NSW</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Boxing Day</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2030-12-26</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>VIC</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
         <is>
           <t>Boxing Day</t>
         </is>

</xml_diff>